<commit_message>
finding bugs, added years to params
</commit_message>
<xml_diff>
--- a/data/share_buildings_2019.xlsx
+++ b/data/share_buildings_2019.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">tabula_code</t>
   </si>
   <si>
-    <t xml:space="preserve">living_space_mio.m2</t>
+    <t xml:space="preserve">living_space_mio.m2_2019</t>
   </si>
   <si>
     <t xml:space="preserve">DE.N.SFH.01.Gen.ReEx.001.001</t>
@@ -870,13 +870,17 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="29" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -983,2038 +987,2038 @@
   </sheetPr>
   <dimension ref="A1:B319"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C100" activeCellId="0" sqref="C100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B134" s="3" t="n">
+      <c r="B134" s="4" t="n">
         <v>37.213861677099</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B135" s="3" t="n">
+      <c r="B135" s="4" t="n">
         <v>109.214594052356</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B136" s="3" t="n">
+      <c r="B136" s="4" t="n">
         <v>121.349548947062</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B137" s="3" t="n">
+      <c r="B137" s="4" t="n">
         <v>93.8436511857279</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B138" s="3" t="n">
+      <c r="B138" s="4" t="n">
         <v>176.36134446973</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="2" t="s">
+      <c r="A139" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B139" s="3" t="n">
+      <c r="B139" s="4" t="n">
         <v>188.496299364436</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B140" s="3" t="n">
+      <c r="B140" s="4" t="n">
         <v>102.787908536808</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B141" s="3" t="n">
+      <c r="B141" s="4" t="n">
         <v>166.329524723198</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B142" s="3" t="n">
+      <c r="B142" s="4" t="n">
         <v>147.640814080142</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B143" s="3" t="n">
+      <c r="B143" s="4" t="n">
         <v>111.197828326183</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="3" t="n">
+      <c r="B144" s="4" t="n">
         <v>67.6597111006131</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="2" t="s">
+      <c r="A145" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B145" s="3" t="n">
+      <c r="B145" s="4" t="n">
         <v>66.3377534243939</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="2" t="s">
+      <c r="A146" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B146" s="3" t="n">
+      <c r="B146" s="4" t="n">
         <v>42.0678436349815</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="2" t="s">
+      <c r="A147" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B147" s="3" t="n">
+      <c r="B147" s="4" t="n">
         <v>61.4837714665114</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="2" t="s">
+      <c r="A148" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B148" s="3" t="n">
+      <c r="B148" s="4" t="n">
         <v>63.9107624454526</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="2" t="s">
+      <c r="A149" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B149" s="3" t="n">
+      <c r="B149" s="4" t="n">
         <v>42.0495989468759</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B150" s="3" t="n">
+      <c r="B150" s="4" t="n">
         <v>79.4270202329877</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="2" t="s">
+      <c r="A151" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B151" s="3" t="n">
+      <c r="B151" s="4" t="n">
         <v>74.7548425722238</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B152" s="3" t="n">
+      <c r="B152" s="4" t="n">
         <v>48.5906476719454</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B153" s="4" t="n">
+      <c r="B153" s="5" t="n">
         <v>12.9439518876866</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="2" t="s">
+      <c r="A154" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B154" s="4" t="n">
+      <c r="B154" s="5" t="n">
         <v>131.866509855807</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="2" t="s">
+      <c r="A155" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B155" s="4" t="n">
+      <c r="B155" s="5" t="n">
         <v>104.360612094473</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2" t="s">
+      <c r="A156" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B156" s="4" t="n">
+      <c r="B156" s="5" t="n">
         <v>101.124624122552</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B157" s="4" t="n">
+      <c r="B157" s="5" t="n">
         <v>182.024323420593</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="2" t="s">
+      <c r="A158" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B158" s="4" t="n">
+      <c r="B158" s="5" t="n">
         <v>136.72049181369</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2" t="s">
+      <c r="A159" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B159" s="4" t="n">
+      <c r="B159" s="5" t="n">
         <v>59.803874057779</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2" t="s">
+      <c r="A160" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B160" s="4" t="n">
+      <c r="B160" s="5" t="n">
         <v>124.279925776322</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="2" t="s">
+      <c r="A161" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B161" s="4" t="n">
+      <c r="B161" s="5" t="n">
         <v>97.1812953438909</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="2" t="s">
+      <c r="A162" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B162" s="4" t="n">
+      <c r="B162" s="5" t="n">
         <v>36.4429857539591</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B163" s="4" t="n">
+      <c r="B163" s="5" t="n">
         <v>29.5283902437851</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2" t="s">
+      <c r="A164" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B164" s="4" t="n">
+      <c r="B164" s="5" t="n">
         <v>6.39107624454526</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="2" t="s">
+      <c r="A165" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B165" s="4" t="n">
+      <c r="B165" s="5" t="n">
         <v>13.752948880667</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="2" t="s">
+      <c r="A166" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B166" s="4" t="n">
+      <c r="B166" s="5" t="n">
         <v>38.1037583693775</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="2" t="s">
+      <c r="A167" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B167" s="4" t="n">
+      <c r="B167" s="5" t="n">
         <v>145.053160841388</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="2" t="s">
+      <c r="A168" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B168" s="4"/>
+      <c r="B168" s="5"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="2" t="s">
+      <c r="A169" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B169" s="4"/>
+      <c r="B169" s="5"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B170" s="4"/>
+      <c r="B170" s="5"/>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B171" s="4"/>
+      <c r="B171" s="5"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="2" t="s">
+      <c r="A172" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B172" s="4"/>
+      <c r="B172" s="5"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="2" t="s">
+      <c r="A173" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B173" s="4"/>
+      <c r="B173" s="5"/>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="2" t="s">
+      <c r="A174" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B174" s="4"/>
+      <c r="B174" s="5"/>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="2" t="s">
+      <c r="A175" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B175" s="4"/>
+      <c r="B175" s="5"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B176" s="4"/>
+      <c r="B176" s="5"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="s">
+      <c r="A177" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B177" s="4"/>
+      <c r="B177" s="5"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2" t="s">
+      <c r="A178" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B178" s="4" t="n">
+      <c r="B178" s="5" t="n">
         <v>8.39764806807266</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="2" t="s">
+      <c r="A179" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B179" s="4" t="n">
+      <c r="B179" s="5" t="n">
         <v>24.6452715041263</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="2" t="s">
+      <c r="A180" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B180" s="4" t="n">
+      <c r="B180" s="5" t="n">
         <v>27.3836350045848</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="2" t="s">
+      <c r="A181" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B181" s="4" t="n">
+      <c r="B181" s="5" t="n">
         <v>21.1766777368789</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="2" t="s">
+      <c r="A182" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B182" s="4" t="n">
+      <c r="B182" s="5" t="n">
         <v>39.7975495399965</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="2" t="s">
+      <c r="A183" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B183" s="4" t="n">
+      <c r="B183" s="5" t="n">
         <v>42.535913040455</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="2" t="s">
+      <c r="A184" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B184" s="4" t="n">
+      <c r="B184" s="5" t="n">
         <v>6.09323564486258</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="2" t="s">
+      <c r="A185" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B185" s="4" t="n">
+      <c r="B185" s="5" t="n">
         <v>9.85996313441399</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="2" t="s">
+      <c r="A186" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B186" s="4" t="n">
+      <c r="B186" s="5" t="n">
         <v>8.75210210807534</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="2" t="s">
+      <c r="A187" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B187" s="4" t="n">
+      <c r="B187" s="5" t="n">
         <v>6.59177310671497</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="2" t="s">
+      <c r="A188" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B188" s="4" t="n">
+      <c r="B188" s="5" t="n">
         <v>12.6562082332761</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="2" t="s">
+      <c r="A189" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B189" s="4" t="n">
+      <c r="B189" s="5" t="n">
         <v>14.969720469173</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B190" s="4" t="n">
+      <c r="B190" s="5" t="n">
         <v>9.49299346825605</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="2" t="s">
+      <c r="A191" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B191" s="4" t="n">
+      <c r="B191" s="5" t="n">
         <v>13.8743750689896</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B192" s="4" t="n">
+      <c r="B192" s="5" t="n">
         <v>14.4220477690813</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="2" t="s">
+      <c r="A193" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B193" s="4" t="n">
+      <c r="B193" s="5" t="n">
         <v>2.49268730926196</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="2" t="s">
+      <c r="A194" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B194" s="4" t="n">
+      <c r="B194" s="5" t="n">
         <v>4.70840936193927</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="2" t="s">
+      <c r="A195" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B195" s="4" t="n">
+      <c r="B195" s="5" t="n">
         <v>4.4314441053546</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="2" t="s">
+      <c r="A196" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B196" s="4" t="n">
+      <c r="B196" s="5" t="n">
         <v>2.88043866848049</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="2" t="s">
+      <c r="A197" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B197" s="4" t="n">
+      <c r="B197" s="5" t="n">
         <v>2.92092106715571</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="2" t="s">
+      <c r="A198" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B198" s="4" t="n">
+      <c r="B198" s="5" t="n">
         <v>29.7568833716488</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="2" t="s">
+      <c r="A199" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B199" s="4" t="n">
+      <c r="B199" s="5" t="n">
         <v>23.5499261039429</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="2" t="s">
+      <c r="A200" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B200" s="4" t="n">
+      <c r="B200" s="5" t="n">
         <v>22.819695837154</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="2" t="s">
+      <c r="A201" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B201" s="4" t="n">
+      <c r="B201" s="5" t="n">
         <v>41.0754525068771</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="2" t="s">
+      <c r="A202" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B202" s="4" t="n">
+      <c r="B202" s="5" t="n">
         <v>30.8522287718322</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="2" t="s">
+      <c r="A203" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B203" s="4" t="n">
+      <c r="B203" s="5" t="n">
         <v>3.54515528428368</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="2" t="s">
+      <c r="A204" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B204" s="4" t="n">
+      <c r="B204" s="5" t="n">
         <v>7.36727582515203</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="2" t="s">
+      <c r="A205" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B205" s="4" t="n">
+      <c r="B205" s="5" t="n">
         <v>5.76087733696098</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="2" t="s">
+      <c r="A206" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B206" s="4" t="n">
+      <c r="B206" s="5" t="n">
         <v>2.16032900136037</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="2" t="s">
+      <c r="A207" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B207" s="4" t="n">
+      <c r="B207" s="5" t="n">
         <v>6.66335118444896</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="2" t="s">
+      <c r="A208" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B208" s="4" t="n">
+      <c r="B208" s="5" t="n">
         <v>1.44220477690813</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="2" t="s">
+      <c r="A209" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B209" s="4" t="n">
+      <c r="B209" s="5" t="n">
         <v>3.10347863385294</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="2" t="s">
+      <c r="A210" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B210" s="4" t="n">
+      <c r="B210" s="5" t="n">
         <v>8.59846139143962</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="2" t="s">
+      <c r="A211" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B211" s="4" t="n">
+      <c r="B211" s="5" t="n">
         <v>32.7325717088137</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="2" t="s">
+      <c r="A212" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B212" s="4"/>
+      <c r="B212" s="5"/>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="2" t="s">
+      <c r="A213" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B213" s="4"/>
+      <c r="B213" s="5"/>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="2" t="s">
+      <c r="A214" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B214" s="4"/>
+      <c r="B214" s="5"/>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="2" t="s">
+      <c r="A215" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B215" s="4"/>
+      <c r="B215" s="5"/>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="2" t="s">
+      <c r="A216" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B216" s="4"/>
+      <c r="B216" s="5"/>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="2" t="s">
+      <c r="A217" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B217" s="4"/>
+      <c r="B217" s="5"/>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="2" t="s">
+      <c r="A218" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B218" s="4"/>
+      <c r="B218" s="5"/>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="2" t="s">
+      <c r="A219" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B219" s="4"/>
+      <c r="B219" s="5"/>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="2" t="s">
+      <c r="A220" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B220" s="4"/>
+      <c r="B220" s="5"/>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="2" t="s">
+      <c r="A221" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B221" s="4"/>
+      <c r="B221" s="5"/>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="2" t="s">
+      <c r="A222" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B222" s="4" t="n">
+      <c r="B222" s="5" t="n">
         <v>0.441981477266982</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="2" t="s">
+      <c r="A223" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B223" s="4" t="n">
+      <c r="B223" s="5" t="n">
         <v>1.29711955284875</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="2" t="s">
+      <c r="A224" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B224" s="4" t="n">
+      <c r="B224" s="5" t="n">
         <v>1.44124394760973</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="2" t="s">
+      <c r="A225" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B225" s="4" t="n">
+      <c r="B225" s="5" t="n">
         <v>1.11456198615152</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="2" t="s">
+      <c r="A226" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B226" s="4" t="n">
+      <c r="B226" s="5" t="n">
         <v>2.09460787052613</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="2" t="s">
+      <c r="A227" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B227" s="4" t="n">
+      <c r="B227" s="5" t="n">
         <v>2.23873226528711</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="2" t="s">
+      <c r="A228" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B228" s="4" t="n">
+      <c r="B228" s="5" t="n">
         <v>1.52330891121564</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="2" t="s">
+      <c r="A229" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B229" s="4" t="n">
+      <c r="B229" s="5" t="n">
         <v>2.4649907836035</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="2" t="s">
+      <c r="A230" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B230" s="4" t="n">
+      <c r="B230" s="5" t="n">
         <v>2.18802552701883</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="2" t="s">
+      <c r="A231" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B231" s="4" t="n">
+      <c r="B231" s="5" t="n">
         <v>1.64794327667874</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="2" t="s">
+      <c r="A232" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B232" s="4" t="n">
+      <c r="B232" s="5" t="n">
         <v>0.778271731709252</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="2" t="s">
+      <c r="A233" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B233" s="4" t="n">
+      <c r="B233" s="5" t="n">
         <v>0.787880024693317</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="2" t="s">
+      <c r="A234" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B234" s="4" t="n">
+      <c r="B234" s="5" t="n">
         <v>0.499631235171372</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="2" t="s">
+      <c r="A235" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B235" s="4" t="n">
+      <c r="B235" s="5" t="n">
         <v>0.730230266788928</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="2" t="s">
+      <c r="A236" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B236" s="4" t="n">
+      <c r="B236" s="5" t="n">
         <v>0.759055145741122</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="2" t="s">
+      <c r="A237" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B237" s="4" t="n">
+      <c r="B237" s="5" t="n">
         <v>0.623171827315491</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="2" t="s">
+      <c r="A238" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B238" s="4" t="n">
+      <c r="B238" s="5" t="n">
         <v>1.17710234048482</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="2" t="s">
+      <c r="A239" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B239" s="4" t="n">
+      <c r="B239" s="5" t="n">
         <v>1.10786102633865</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="2" t="s">
+      <c r="A240" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B240" s="4" t="n">
+      <c r="B240" s="5" t="n">
         <v>0.720109667120123</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="2" t="s">
+      <c r="A241" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B241" s="4" t="n">
+      <c r="B241" s="5" t="n">
         <v>0.153732687745037</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="2" t="s">
+      <c r="A242" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B242" s="4" t="n">
+      <c r="B242" s="5" t="n">
         <v>1.56615175640257</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="2" t="s">
+      <c r="A243" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B243" s="4" t="n">
+      <c r="B243" s="5" t="n">
         <v>1.23946979494436</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="2" t="s">
+      <c r="A244" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B244" s="4" t="n">
+      <c r="B244" s="5" t="n">
         <v>1.2010366230081</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="2" t="s">
+      <c r="A245" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B245" s="4" t="n">
+      <c r="B245" s="5" t="n">
         <v>2.16186592141459</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="2" t="s">
+      <c r="A246" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B246" s="4" t="n">
+      <c r="B246" s="5" t="n">
         <v>1.62380151430696</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="2" t="s">
+      <c r="A247" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B247" s="4" t="n">
+      <c r="B247" s="5" t="n">
         <v>0.88628882107092</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="2" t="s">
+      <c r="A248" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B248" s="4" t="n">
+      <c r="B248" s="5" t="n">
         <v>1.84181895628801</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="2" t="s">
+      <c r="A249" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B249" s="4" t="n">
+      <c r="B249" s="5" t="n">
         <v>1.44021933424025</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="2" t="s">
+      <c r="A250" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B250" s="4" t="n">
+      <c r="B250" s="5" t="n">
         <v>0.540082250340092</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="2" t="s">
+      <c r="A251" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B251" s="4" t="n">
+      <c r="B251" s="5" t="n">
         <v>0.350702693918366</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="2" t="s">
+      <c r="A252" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B252" s="4" t="n">
+      <c r="B252" s="5" t="n">
         <v>0.0759055145741122</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="2" t="s">
+      <c r="A253" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B253" s="4" t="n">
+      <c r="B253" s="5" t="n">
         <v>0.163340980729102</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="2" t="s">
+      <c r="A254" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B254" s="4" t="n">
+      <c r="B254" s="5" t="n">
         <v>0.452550599549454</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="2" t="s">
+      <c r="A255" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B255" s="4" t="n">
+      <c r="B255" s="5" t="n">
         <v>1.72276693204283</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="2" t="s">
+      <c r="A256" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B256" s="4"/>
+      <c r="B256" s="5"/>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="2" t="s">
+      <c r="A257" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B257" s="4"/>
+      <c r="B257" s="5"/>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="2" t="s">
+      <c r="A258" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B258" s="4"/>
+      <c r="B258" s="5"/>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="2" t="s">
+      <c r="A259" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B259" s="4"/>
+      <c r="B259" s="5"/>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="2" t="s">
+      <c r="A260" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B260" s="4"/>
+      <c r="B260" s="5"/>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="2" t="s">
+      <c r="A261" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B261" s="4"/>
+      <c r="B261" s="5"/>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="2" t="s">
+      <c r="A262" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B262" s="4"/>
+      <c r="B262" s="5"/>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="2" t="s">
+      <c r="A263" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B263" s="4"/>
+      <c r="B263" s="5"/>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="2" t="s">
+      <c r="A264" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B264" s="4"/>
+      <c r="B264" s="5"/>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="2" t="s">
+      <c r="A265" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B265" s="4"/>
+      <c r="B265" s="5"/>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="2" t="s">
+      <c r="A266" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B266" s="4" t="n">
+      <c r="B266" s="5" t="n">
         <v>12.91075</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="2" t="s">
+      <c r="A267" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B267" s="4" t="n">
+      <c r="B267" s="5" t="n">
         <v>42.035</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="2" t="s">
+      <c r="A268" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B268" s="4" t="n">
+      <c r="B268" s="5" t="n">
         <v>5.10425</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="2" t="s">
+      <c r="A269" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B269" s="4"/>
+      <c r="B269" s="5"/>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="2" t="s">
+      <c r="A270" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B270" s="4"/>
+      <c r="B270" s="5"/>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="2" t="s">
+      <c r="A271" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B271" s="4"/>
+      <c r="B271" s="5"/>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="2" t="s">
+      <c r="A272" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B272" s="4"/>
+      <c r="B272" s="5"/>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="2" t="s">
+      <c r="A273" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B273" s="4"/>
+      <c r="B273" s="5"/>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="2" t="s">
+      <c r="A274" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B274" s="4"/>
+      <c r="B274" s="5"/>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="2" t="s">
+      <c r="A275" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B275" s="4" t="n">
+      <c r="B275" s="5" t="n">
         <v>1.92812</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="2" t="s">
+      <c r="A276" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B276" s="4" t="n">
+      <c r="B276" s="5" t="n">
         <v>6.2776</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="2" t="s">
+      <c r="A277" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B277" s="4" t="n">
+      <c r="B277" s="5" t="n">
         <v>0.76228</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="2" t="s">
+      <c r="A278" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B278" s="4"/>
+      <c r="B278" s="5"/>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="2" t="s">
+      <c r="A279" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B279" s="4"/>
+      <c r="B279" s="5"/>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="2" t="s">
+      <c r="A280" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B280" s="4"/>
+      <c r="B280" s="5"/>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="2" t="s">
+      <c r="A281" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B281" s="4"/>
+      <c r="B281" s="5"/>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="2" t="s">
+      <c r="A282" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B282" s="4"/>
+      <c r="B282" s="5"/>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="2" t="s">
+      <c r="A283" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B283" s="4"/>
+      <c r="B283" s="5"/>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="2" t="s">
+      <c r="A284" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B284" s="4" t="n">
+      <c r="B284" s="5" t="n">
         <v>6.640275</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="2" t="s">
+      <c r="A285" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B285" s="4" t="n">
+      <c r="B285" s="5" t="n">
         <v>21.6195</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="2" t="s">
+      <c r="A286" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B286" s="4" t="n">
+      <c r="B286" s="5" t="n">
         <v>2.625225</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="2" t="s">
+      <c r="A287" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B287" s="4"/>
+      <c r="B287" s="5"/>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="2" t="s">
+      <c r="A288" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B288" s="4"/>
+      <c r="B288" s="5"/>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="2" t="s">
+      <c r="A289" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B289" s="4"/>
+      <c r="B289" s="5"/>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="2" t="s">
+      <c r="A290" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B290" s="4"/>
+      <c r="B290" s="5"/>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="2" t="s">
+      <c r="A291" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B291" s="4"/>
+      <c r="B291" s="5"/>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="2" t="s">
+      <c r="A292" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B292" s="4"/>
+      <c r="B292" s="5"/>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="2" t="s">
+      <c r="A293" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B293" s="4" t="n">
+      <c r="B293" s="5" t="n">
         <v>13.4147766797304</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="2" t="s">
+      <c r="A294" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B294" s="4" t="n">
+      <c r="B294" s="5" t="n">
         <v>43.6760170967968</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="2" t="s">
+      <c r="A295" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B295" s="4" t="n">
+      <c r="B295" s="5" t="n">
         <v>5.3035163617539</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="2" t="s">
+      <c r="A296" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B296" s="4"/>
+      <c r="B296" s="5"/>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="2" t="s">
+      <c r="A297" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B297" s="4"/>
+      <c r="B297" s="5"/>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="2" t="s">
+      <c r="A298" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B298" s="4"/>
+      <c r="B298" s="5"/>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="2" t="s">
+      <c r="A299" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B299" s="4"/>
+      <c r="B299" s="5"/>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="2" t="s">
+      <c r="A300" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B300" s="4"/>
+      <c r="B300" s="5"/>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="2" t="s">
+      <c r="A301" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B301" s="4"/>
+      <c r="B301" s="5"/>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="2" t="s">
+      <c r="A302" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B302" s="4" t="n">
+      <c r="B302" s="5" t="n">
         <v>2.19893802232925</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="2" t="s">
+      <c r="A303" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B303" s="4" t="n">
+      <c r="B303" s="5" t="n">
         <v>7.1593330959557</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="2" t="s">
+      <c r="A304" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B304" s="4" t="n">
+      <c r="B304" s="5" t="n">
         <v>0.869347590223192</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="2" t="s">
+      <c r="A305" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B305" s="4"/>
+      <c r="B305" s="5"/>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="2" t="s">
+      <c r="A306" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B306" s="4"/>
+      <c r="B306" s="5"/>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="2" t="s">
+      <c r="A307" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B307" s="4"/>
+      <c r="B307" s="5"/>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="2" t="s">
+      <c r="A308" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B308" s="4"/>
+      <c r="B308" s="5"/>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="2" t="s">
+      <c r="A309" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B309" s="4"/>
+      <c r="B309" s="5"/>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="2" t="s">
+      <c r="A310" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B310" s="4"/>
+      <c r="B310" s="5"/>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="2" t="s">
+      <c r="A311" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B311" s="4" t="n">
+      <c r="B311" s="5" t="n">
         <v>10.4925313447296</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="2" t="s">
+      <c r="A312" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B312" s="4" t="n">
+      <c r="B312" s="5" t="n">
         <v>34.1617298072475</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="2" t="s">
+      <c r="A313" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B313" s="4" t="n">
+      <c r="B313" s="5" t="n">
         <v>4.14821004802291</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="2" t="s">
+      <c r="A314" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B314" s="4"/>
+      <c r="B314" s="5"/>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="2" t="s">
+      <c r="A315" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B315" s="4"/>
+      <c r="B315" s="5"/>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="2" t="s">
+      <c r="A316" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B316" s="4"/>
+      <c r="B316" s="5"/>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="2" t="s">
+      <c r="A317" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B317" s="4"/>
+      <c r="B317" s="5"/>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="2" t="s">
+      <c r="A318" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B318" s="4"/>
+      <c r="B318" s="5"/>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="2" t="s">
+      <c r="A319" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B319" s="4"/>
+      <c r="B319" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>